<commit_message>
Cleaning Repository for Publishing
</commit_message>
<xml_diff>
--- a/SapeloIR/Data/Botsch_Sapelo_Snail_MASTER.xlsx
+++ b/SapeloIR/Data/Botsch_Sapelo_Snail_MASTER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcbot\Desktop\Research\Sapelo2018\SapeloIR\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D288232-6807-4269-94A6-8AA81EB811A9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4C8EE4-DDC4-4E65-8788-24EC0B3631B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19070" windowHeight="6690" activeTab="2" xr2:uid="{7C658811-3A91-40C3-90DB-53D0813241B5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19070" windowHeight="6690" xr2:uid="{7C658811-3A91-40C3-90DB-53D0813241B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="77">
   <si>
     <t>Snail</t>
   </si>
@@ -108,12 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">forgot to measure </t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>long</t>
   </si>
   <si>
     <t>Sheet</t>
@@ -197,19 +191,10 @@
     <t>The location from the creek where the subplot is located</t>
   </si>
   <si>
-    <t>latitude of the subplot</t>
-  </si>
-  <si>
-    <t>longitude of the subplot</t>
-  </si>
-  <si>
     <t>Number of Spartina stalks of the subplot</t>
   </si>
   <si>
     <t>Height of a Spartina stalk of the subplot in centimeters</t>
-  </si>
-  <si>
-    <t>Decimal Degrees</t>
   </si>
   <si>
     <t>##</t>
@@ -644,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5B85AB-A5E8-4E7E-AA98-B5D0920B5C66}">
-  <dimension ref="A3:E24"/>
+  <dimension ref="A3:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,36 +645,36 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -698,13 +683,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -713,13 +698,13 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -728,13 +713,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -743,13 +728,13 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -758,13 +743,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -773,13 +758,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -788,13 +773,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -803,28 +788,28 @@
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -833,13 +818,13 @@
         <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -848,140 +833,114 @@
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3405,7 +3364,7 @@
         <v>22</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F92" t="s">
         <v>23</v>
@@ -3417,7 +3376,7 @@
         <v>23</v>
       </c>
       <c r="I92" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -3434,7 +3393,7 @@
         <v>22</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F93" t="s">
         <v>23</v>
@@ -3446,7 +3405,7 @@
         <v>23</v>
       </c>
       <c r="I93" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -3463,7 +3422,7 @@
         <v>22</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F94" t="s">
         <v>23</v>
@@ -3475,7 +3434,7 @@
         <v>23</v>
       </c>
       <c r="I94" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -3492,7 +3451,7 @@
         <v>22</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F95" t="s">
         <v>23</v>
@@ -3518,7 +3477,7 @@
         <v>22</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F96" t="s">
         <v>23</v>
@@ -3544,7 +3503,7 @@
         <v>22</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F97" t="s">
         <v>23</v>
@@ -3570,7 +3529,7 @@
         <v>22</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F98" t="s">
         <v>23</v>
@@ -3596,7 +3555,7 @@
         <v>22</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F99" t="s">
         <v>23</v>
@@ -3622,7 +3581,7 @@
         <v>22</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F100" t="s">
         <v>23</v>
@@ -3648,7 +3607,7 @@
         <v>22</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F101" t="s">
         <v>23</v>
@@ -3674,7 +3633,7 @@
         <v>22</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F102" t="s">
         <v>23</v>
@@ -3700,7 +3659,7 @@
         <v>22</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F103" t="s">
         <v>23</v>
@@ -3726,7 +3685,7 @@
         <v>22</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F104" t="s">
         <v>23</v>
@@ -3752,7 +3711,7 @@
         <v>22</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F105" t="s">
         <v>23</v>
@@ -3778,7 +3737,7 @@
         <v>22</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F106" t="s">
         <v>23</v>
@@ -3804,7 +3763,7 @@
         <v>22</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F107" t="s">
         <v>23</v>
@@ -3830,7 +3789,7 @@
         <v>22</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F108" t="s">
         <v>23</v>
@@ -3856,7 +3815,7 @@
         <v>22</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F109" t="s">
         <v>23</v>
@@ -3868,7 +3827,7 @@
         <v>23</v>
       </c>
       <c r="I109" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
@@ -3885,7 +3844,7 @@
         <v>22</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F110" t="s">
         <v>23</v>
@@ -3911,7 +3870,7 @@
         <v>22</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F111" t="s">
         <v>23</v>
@@ -3937,7 +3896,7 @@
         <v>22</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F112" t="s">
         <v>23</v>
@@ -3963,7 +3922,7 @@
         <v>22</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F113" t="s">
         <v>23</v>
@@ -3989,7 +3948,7 @@
         <v>22</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F114" t="s">
         <v>23</v>
@@ -4015,7 +3974,7 @@
         <v>22</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F115" t="s">
         <v>23</v>
@@ -4041,7 +4000,7 @@
         <v>22</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F116" t="s">
         <v>23</v>
@@ -4067,7 +4026,7 @@
         <v>22</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F117" t="s">
         <v>23</v>
@@ -4093,7 +4052,7 @@
         <v>22</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F118" t="s">
         <v>23</v>
@@ -4119,7 +4078,7 @@
         <v>22</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F119" t="s">
         <v>23</v>
@@ -4145,7 +4104,7 @@
         <v>22</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F120" t="s">
         <v>23</v>
@@ -4171,7 +4130,7 @@
         <v>22</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F121" t="s">
         <v>23</v>
@@ -4197,7 +4156,7 @@
         <v>22</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F122" t="s">
         <v>23</v>
@@ -4223,7 +4182,7 @@
         <v>22</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F123" t="s">
         <v>23</v>
@@ -4249,7 +4208,7 @@
         <v>22</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F124" t="s">
         <v>23</v>
@@ -4275,7 +4234,7 @@
         <v>22</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F125" t="s">
         <v>23</v>
@@ -4301,7 +4260,7 @@
         <v>22</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F126" t="s">
         <v>23</v>
@@ -4327,7 +4286,7 @@
         <v>22</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F127" t="s">
         <v>23</v>
@@ -4353,7 +4312,7 @@
         <v>22</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F128" t="s">
         <v>23</v>
@@ -4379,7 +4338,7 @@
         <v>22</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F129" t="s">
         <v>23</v>
@@ -4405,7 +4364,7 @@
         <v>22</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F130" t="s">
         <v>23</v>
@@ -4431,7 +4390,7 @@
         <v>22</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F131" t="s">
         <v>23</v>
@@ -4457,7 +4416,7 @@
         <v>22</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F132" t="s">
         <v>23</v>
@@ -4483,7 +4442,7 @@
         <v>22</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F133" t="s">
         <v>23</v>
@@ -4509,7 +4468,7 @@
         <v>22</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F134" t="s">
         <v>23</v>
@@ -4535,7 +4494,7 @@
         <v>22</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F135" t="s">
         <v>23</v>
@@ -4561,7 +4520,7 @@
         <v>22</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F136" t="s">
         <v>23</v>
@@ -4587,7 +4546,7 @@
         <v>22</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F137" t="s">
         <v>23</v>
@@ -4613,7 +4572,7 @@
         <v>22</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F138" t="s">
         <v>23</v>
@@ -4639,7 +4598,7 @@
         <v>22</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F139" t="s">
         <v>23</v>
@@ -4665,7 +4624,7 @@
         <v>22</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F140" t="s">
         <v>23</v>
@@ -4677,7 +4636,7 @@
         <v>23</v>
       </c>
       <c r="I140" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.35">
@@ -4694,7 +4653,7 @@
         <v>22</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F141" t="s">
         <v>23</v>
@@ -4720,7 +4679,7 @@
         <v>22</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F142" t="s">
         <v>23</v>
@@ -4746,7 +4705,7 @@
         <v>22</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F143" t="s">
         <v>23</v>
@@ -4772,7 +4731,7 @@
         <v>22</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F144" t="s">
         <v>23</v>
@@ -4798,7 +4757,7 @@
         <v>22</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F145" t="s">
         <v>23</v>
@@ -4824,7 +4783,7 @@
         <v>22</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F146" t="s">
         <v>23</v>
@@ -4850,7 +4809,7 @@
         <v>22</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F147" t="s">
         <v>23</v>
@@ -4876,7 +4835,7 @@
         <v>22</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F148" t="s">
         <v>23</v>
@@ -4902,7 +4861,7 @@
         <v>22</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F149" t="s">
         <v>23</v>
@@ -4928,7 +4887,7 @@
         <v>22</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F150" t="s">
         <v>23</v>
@@ -4954,7 +4913,7 @@
         <v>22</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F151" t="s">
         <v>23</v>
@@ -4980,7 +4939,7 @@
         <v>22</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F152" t="s">
         <v>23</v>
@@ -5006,7 +4965,7 @@
         <v>22</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F153" t="s">
         <v>23</v>
@@ -5032,7 +4991,7 @@
         <v>22</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F154" t="s">
         <v>23</v>
@@ -5058,7 +5017,7 @@
         <v>22</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F155" t="s">
         <v>23</v>
@@ -5084,7 +5043,7 @@
         <v>22</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F156" t="s">
         <v>23</v>
@@ -5110,7 +5069,7 @@
         <v>22</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F157" t="s">
         <v>23</v>
@@ -5136,7 +5095,7 @@
         <v>22</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F158" t="s">
         <v>23</v>
@@ -5162,7 +5121,7 @@
         <v>22</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F159" t="s">
         <v>23</v>
@@ -5188,7 +5147,7 @@
         <v>22</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F160" t="s">
         <v>23</v>
@@ -5214,7 +5173,7 @@
         <v>22</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F161" t="s">
         <v>23</v>
@@ -5240,7 +5199,7 @@
         <v>22</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F162" t="s">
         <v>23</v>
@@ -5266,7 +5225,7 @@
         <v>22</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F163" t="s">
         <v>23</v>
@@ -5292,7 +5251,7 @@
         <v>22</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F164" t="s">
         <v>23</v>
@@ -5318,7 +5277,7 @@
         <v>22</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F165" t="s">
         <v>23</v>
@@ -5344,7 +5303,7 @@
         <v>22</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F166" t="s">
         <v>23</v>
@@ -5370,7 +5329,7 @@
         <v>22</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F167" t="s">
         <v>23</v>
@@ -5396,7 +5355,7 @@
         <v>22</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F168" t="s">
         <v>23</v>
@@ -5422,7 +5381,7 @@
         <v>22</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F169" t="s">
         <v>23</v>
@@ -5448,7 +5407,7 @@
         <v>22</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F170" t="s">
         <v>23</v>
@@ -5474,7 +5433,7 @@
         <v>22</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F171" t="s">
         <v>23</v>
@@ -5500,7 +5459,7 @@
         <v>22</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F172" t="s">
         <v>23</v>
@@ -5526,7 +5485,7 @@
         <v>22</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F173" t="s">
         <v>23</v>
@@ -5552,7 +5511,7 @@
         <v>22</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F174" t="s">
         <v>23</v>
@@ -5578,7 +5537,7 @@
         <v>22</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F175" t="s">
         <v>23</v>
@@ -5604,7 +5563,7 @@
         <v>22</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F176" t="s">
         <v>23</v>
@@ -5630,7 +5589,7 @@
         <v>22</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F177" t="s">
         <v>23</v>
@@ -5656,7 +5615,7 @@
         <v>22</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F178" t="s">
         <v>23</v>
@@ -5682,7 +5641,7 @@
         <v>22</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F179" t="s">
         <v>23</v>
@@ -5708,7 +5667,7 @@
         <v>22</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F180" t="s">
         <v>23</v>
@@ -5734,7 +5693,7 @@
         <v>22</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F181" t="s">
         <v>23</v>
@@ -5760,7 +5719,7 @@
         <v>22</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F182" t="s">
         <v>23</v>
@@ -5783,10 +5742,10 @@
         <v>5</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F183" t="s">
         <v>23</v>
@@ -5809,10 +5768,10 @@
         <v>5</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F184" t="s">
         <v>23</v>
@@ -5835,10 +5794,10 @@
         <v>5</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F185" t="s">
         <v>23</v>
@@ -5861,10 +5820,10 @@
         <v>5</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F186" t="s">
         <v>23</v>
@@ -5887,10 +5846,10 @@
         <v>5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F187" t="s">
         <v>23</v>
@@ -5913,10 +5872,10 @@
         <v>5</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F188" t="s">
         <v>23</v>
@@ -5939,10 +5898,10 @@
         <v>5</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F189" t="s">
         <v>23</v>
@@ -5965,10 +5924,10 @@
         <v>5</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F190" t="s">
         <v>23</v>
@@ -5991,10 +5950,10 @@
         <v>5</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F191" t="s">
         <v>23</v>
@@ -6017,10 +5976,10 @@
         <v>5</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F192" t="s">
         <v>23</v>
@@ -6043,10 +6002,10 @@
         <v>5</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F193" t="s">
         <v>23</v>
@@ -6069,10 +6028,10 @@
         <v>5</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F194" t="s">
         <v>23</v>
@@ -6095,10 +6054,10 @@
         <v>5</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F195" t="s">
         <v>23</v>
@@ -6121,10 +6080,10 @@
         <v>5</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F196" t="s">
         <v>23</v>
@@ -6147,10 +6106,10 @@
         <v>5</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F197" t="s">
         <v>23</v>
@@ -6173,10 +6132,10 @@
         <v>5</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F198" t="s">
         <v>23</v>
@@ -6199,10 +6158,10 @@
         <v>5</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F199" t="s">
         <v>23</v>
@@ -6225,10 +6184,10 @@
         <v>5</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F200" t="s">
         <v>23</v>
@@ -6251,10 +6210,10 @@
         <v>5</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F201" t="s">
         <v>23</v>
@@ -6277,10 +6236,10 @@
         <v>5</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F202" t="s">
         <v>23</v>
@@ -6303,10 +6262,10 @@
         <v>5</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F203" t="s">
         <v>23</v>
@@ -6329,10 +6288,10 @@
         <v>5</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F204" t="s">
         <v>23</v>
@@ -6355,10 +6314,10 @@
         <v>5</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F205" t="s">
         <v>23</v>
@@ -6381,10 +6340,10 @@
         <v>5</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F206" t="s">
         <v>23</v>
@@ -6407,10 +6366,10 @@
         <v>5</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F207" t="s">
         <v>23</v>
@@ -6433,10 +6392,10 @@
         <v>5</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F208" t="s">
         <v>23</v>
@@ -6459,10 +6418,10 @@
         <v>5</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F209" t="s">
         <v>23</v>
@@ -6485,10 +6444,10 @@
         <v>5</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F210" t="s">
         <v>23</v>
@@ -6511,10 +6470,10 @@
         <v>5</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F211" t="s">
         <v>23</v>
@@ -6537,10 +6496,10 @@
         <v>5</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F212" t="s">
         <v>23</v>
@@ -6563,10 +6522,10 @@
         <v>5</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F213" t="s">
         <v>23</v>
@@ -6589,10 +6548,10 @@
         <v>5</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F214" t="s">
         <v>23</v>
@@ -6615,10 +6574,10 @@
         <v>5</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F215" t="s">
         <v>23</v>
@@ -6641,10 +6600,10 @@
         <v>5</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F216" t="s">
         <v>23</v>
@@ -6667,10 +6626,10 @@
         <v>5</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F217" t="s">
         <v>23</v>
@@ -6693,10 +6652,10 @@
         <v>5</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F218" t="s">
         <v>23</v>
@@ -6719,10 +6678,10 @@
         <v>5</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F219" t="s">
         <v>23</v>
@@ -6745,10 +6704,10 @@
         <v>5</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F220" t="s">
         <v>23</v>
@@ -6771,10 +6730,10 @@
         <v>5</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F221" t="s">
         <v>23</v>
@@ -6797,10 +6756,10 @@
         <v>5</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F222" t="s">
         <v>23</v>
@@ -6823,10 +6782,10 @@
         <v>5</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F223" t="s">
         <v>23</v>
@@ -6849,10 +6808,10 @@
         <v>5</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F224" t="s">
         <v>23</v>
@@ -6875,10 +6834,10 @@
         <v>5</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F225" t="s">
         <v>23</v>
@@ -6890,7 +6849,7 @@
         <v>23</v>
       </c>
       <c r="I225" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.35">
@@ -6904,10 +6863,10 @@
         <v>5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F226" t="s">
         <v>23</v>
@@ -6930,10 +6889,10 @@
         <v>5</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F227" t="s">
         <v>23</v>
@@ -6956,10 +6915,10 @@
         <v>5</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F228" t="s">
         <v>23</v>
@@ -6982,10 +6941,10 @@
         <v>5</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F229" t="s">
         <v>23</v>
@@ -7008,10 +6967,10 @@
         <v>5</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F230" t="s">
         <v>23</v>
@@ -7034,10 +6993,10 @@
         <v>5</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F231" t="s">
         <v>23</v>
@@ -7060,10 +7019,10 @@
         <v>5</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F232" t="s">
         <v>23</v>
@@ -7086,10 +7045,10 @@
         <v>5</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F233" t="s">
         <v>23</v>
@@ -7112,10 +7071,10 @@
         <v>5</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F234" t="s">
         <v>23</v>
@@ -7138,10 +7097,10 @@
         <v>5</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F235" t="s">
         <v>23</v>
@@ -7164,10 +7123,10 @@
         <v>5</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F236" t="s">
         <v>23</v>
@@ -7190,10 +7149,10 @@
         <v>5</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F237" t="s">
         <v>23</v>
@@ -7216,10 +7175,10 @@
         <v>5</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F238" t="s">
         <v>23</v>
@@ -7242,10 +7201,10 @@
         <v>5</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F239" t="s">
         <v>23</v>
@@ -7268,10 +7227,10 @@
         <v>5</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F240" t="s">
         <v>23</v>
@@ -7294,10 +7253,10 @@
         <v>5</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F241" t="s">
         <v>23</v>
@@ -7320,10 +7279,10 @@
         <v>5</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F242" t="s">
         <v>23</v>
@@ -7346,10 +7305,10 @@
         <v>4</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F243" t="s">
         <v>23</v>
@@ -7372,10 +7331,10 @@
         <v>4</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F244" t="s">
         <v>23</v>
@@ -7398,10 +7357,10 @@
         <v>4</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F245" t="s">
         <v>23</v>
@@ -7424,10 +7383,10 @@
         <v>4</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F246" t="s">
         <v>23</v>
@@ -7450,10 +7409,10 @@
         <v>4</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F247" t="s">
         <v>23</v>
@@ -7476,10 +7435,10 @@
         <v>4</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F248" t="s">
         <v>23</v>
@@ -7502,10 +7461,10 @@
         <v>4</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F249" t="s">
         <v>23</v>
@@ -7528,10 +7487,10 @@
         <v>4</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F250" t="s">
         <v>23</v>
@@ -7554,10 +7513,10 @@
         <v>4</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F251" t="s">
         <v>23</v>
@@ -7580,10 +7539,10 @@
         <v>4</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F252" t="s">
         <v>23</v>
@@ -7606,10 +7565,10 @@
         <v>4</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F253" t="s">
         <v>23</v>
@@ -7632,10 +7591,10 @@
         <v>4</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F254" t="s">
         <v>23</v>
@@ -7658,10 +7617,10 @@
         <v>4</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F255" t="s">
         <v>23</v>
@@ -7684,10 +7643,10 @@
         <v>4</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F256" t="s">
         <v>23</v>
@@ -7710,10 +7669,10 @@
         <v>4</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F257" t="s">
         <v>23</v>
@@ -7736,10 +7695,10 @@
         <v>4</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F258" t="s">
         <v>23</v>
@@ -7762,10 +7721,10 @@
         <v>4</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F259" t="s">
         <v>23</v>
@@ -7788,10 +7747,10 @@
         <v>4</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F260" t="s">
         <v>23</v>
@@ -7814,10 +7773,10 @@
         <v>4</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F261" t="s">
         <v>23</v>
@@ -7840,10 +7799,10 @@
         <v>4</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F262" t="s">
         <v>23</v>
@@ -7866,10 +7825,10 @@
         <v>4</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F263" t="s">
         <v>23</v>
@@ -7892,10 +7851,10 @@
         <v>4</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F264" t="s">
         <v>23</v>
@@ -7918,10 +7877,10 @@
         <v>4</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F265" t="s">
         <v>23</v>
@@ -7944,10 +7903,10 @@
         <v>4</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F266" t="s">
         <v>23</v>
@@ -7970,10 +7929,10 @@
         <v>4</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F267" t="s">
         <v>23</v>
@@ -7996,10 +7955,10 @@
         <v>4</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F268" t="s">
         <v>23</v>
@@ -8022,10 +7981,10 @@
         <v>4</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F269" t="s">
         <v>23</v>
@@ -8048,10 +8007,10 @@
         <v>4</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F270" t="s">
         <v>23</v>
@@ -8074,10 +8033,10 @@
         <v>4</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F271" t="s">
         <v>23</v>
@@ -8100,10 +8059,10 @@
         <v>4</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F272" t="s">
         <v>23</v>
@@ -8126,10 +8085,10 @@
         <v>4</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F273" t="s">
         <v>23</v>
@@ -8152,10 +8111,10 @@
         <v>4</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F274" t="s">
         <v>23</v>
@@ -8178,10 +8137,10 @@
         <v>4</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F275" t="s">
         <v>23</v>
@@ -8204,10 +8163,10 @@
         <v>4</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F276" t="s">
         <v>23</v>
@@ -8230,10 +8189,10 @@
         <v>4</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F277" t="s">
         <v>23</v>
@@ -8256,10 +8215,10 @@
         <v>4</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F278" t="s">
         <v>23</v>
@@ -8282,10 +8241,10 @@
         <v>4</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F279" t="s">
         <v>23</v>
@@ -8308,10 +8267,10 @@
         <v>4</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F280" t="s">
         <v>23</v>
@@ -8334,10 +8293,10 @@
         <v>4</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F281" t="s">
         <v>23</v>
@@ -8360,10 +8319,10 @@
         <v>4</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F282" t="s">
         <v>23</v>
@@ -8386,10 +8345,10 @@
         <v>4</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F283" t="s">
         <v>23</v>
@@ -8412,10 +8371,10 @@
         <v>4</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F284" t="s">
         <v>23</v>
@@ -8438,10 +8397,10 @@
         <v>4</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F285" t="s">
         <v>23</v>
@@ -8464,10 +8423,10 @@
         <v>4</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F286" t="s">
         <v>23</v>
@@ -8490,10 +8449,10 @@
         <v>4</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F287" t="s">
         <v>23</v>
@@ -8516,10 +8475,10 @@
         <v>4</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F288" t="s">
         <v>23</v>
@@ -8542,10 +8501,10 @@
         <v>4</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F289" t="s">
         <v>23</v>
@@ -8568,10 +8527,10 @@
         <v>4</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F290" t="s">
         <v>23</v>
@@ -8594,10 +8553,10 @@
         <v>4</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F291" t="s">
         <v>23</v>
@@ -8620,10 +8579,10 @@
         <v>4</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F292" t="s">
         <v>23</v>
@@ -8646,10 +8605,10 @@
         <v>4</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F293" t="s">
         <v>23</v>
@@ -8672,10 +8631,10 @@
         <v>4</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F294" t="s">
         <v>23</v>
@@ -8698,10 +8657,10 @@
         <v>4</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F295" t="s">
         <v>23</v>
@@ -8724,10 +8683,10 @@
         <v>4</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F296" t="s">
         <v>23</v>
@@ -8750,10 +8709,10 @@
         <v>4</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F297" t="s">
         <v>23</v>
@@ -8776,10 +8735,10 @@
         <v>4</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F298" t="s">
         <v>23</v>
@@ -8802,10 +8761,10 @@
         <v>4</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F299" t="s">
         <v>23</v>
@@ -8828,10 +8787,10 @@
         <v>4</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F300" t="s">
         <v>23</v>
@@ -8854,10 +8813,10 @@
         <v>4</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F301" t="s">
         <v>23</v>
@@ -8880,10 +8839,10 @@
         <v>4</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F302" t="s">
         <v>23</v>
@@ -8903,19 +8862,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2A9E7B-D748-4D55-9611-E438779763B5}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -8923,25 +8881,19 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8949,16 +8901,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="E2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8966,16 +8918,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3">
+        <v>61</v>
+      </c>
+      <c r="D3">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="E3">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -8983,16 +8935,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4">
+        <v>62</v>
+      </c>
+      <c r="D4">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="E4">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9000,16 +8952,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -9017,16 +8969,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6">
+        <v>61</v>
+      </c>
+      <c r="D6">
         <v>33</v>
       </c>
-      <c r="G6">
+      <c r="E6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -9034,16 +8986,16 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7">
+        <v>62</v>
+      </c>
+      <c r="D7">
         <v>30</v>
       </c>
-      <c r="G7">
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -9051,16 +9003,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="D8">
         <v>13</v>
       </c>
-      <c r="G8">
+      <c r="E8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -9068,16 +9020,16 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9">
+        <v>61</v>
+      </c>
+      <c r="D9">
         <v>13</v>
       </c>
-      <c r="G9">
+      <c r="E9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -9085,16 +9037,16 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10">
+        <v>62</v>
+      </c>
+      <c r="D10">
         <v>15</v>
       </c>
-      <c r="G10">
+      <c r="E10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -9102,16 +9054,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="D11">
         <v>16</v>
       </c>
-      <c r="G11">
+      <c r="E11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -9119,19 +9071,19 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12">
+        <v>61</v>
+      </c>
+      <c r="D12">
         <v>28</v>
       </c>
-      <c r="G12">
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
@@ -9139,16 +9091,16 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13">
+        <v>62</v>
+      </c>
+      <c r="D13">
         <v>55</v>
       </c>
-      <c r="G13">
+      <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -9156,19 +9108,19 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14">
+        <v>60</v>
+      </c>
+      <c r="D14">
         <v>15</v>
       </c>
-      <c r="G14">
+      <c r="E14">
         <v>16</v>
       </c>
-      <c r="H14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -9176,19 +9128,19 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15">
+        <v>61</v>
+      </c>
+      <c r="D15">
         <v>12</v>
       </c>
-      <c r="G15">
+      <c r="E15">
         <v>10</v>
       </c>
-      <c r="H15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -9196,19 +9148,19 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16">
+        <v>62</v>
+      </c>
+      <c r="D16">
         <v>17</v>
       </c>
-      <c r="G16">
+      <c r="E16">
         <v>7</v>
       </c>
-      <c r="H16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -9216,19 +9168,19 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17">
-        <v>23</v>
-      </c>
-      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="E17">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -9236,19 +9188,19 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18">
+        <v>61</v>
+      </c>
+      <c r="D18">
         <v>13</v>
       </c>
-      <c r="G18">
+      <c r="E18">
         <v>3</v>
       </c>
-      <c r="H18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -9256,19 +9208,19 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19">
+        <v>62</v>
+      </c>
+      <c r="D19">
         <v>17</v>
       </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5</v>
       </c>
@@ -9276,16 +9228,16 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="D20">
         <v>13</v>
       </c>
-      <c r="G20">
+      <c r="E20">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5</v>
       </c>
@@ -9293,16 +9245,16 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21">
-        <v>11</v>
-      </c>
-      <c r="G21">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5</v>
       </c>
@@ -9310,16 +9262,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22">
-        <v>22</v>
-      </c>
-      <c r="G22">
+        <v>62</v>
+      </c>
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5</v>
       </c>
@@ -9327,16 +9279,16 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23">
+        <v>60</v>
+      </c>
+      <c r="D23">
         <v>12</v>
       </c>
-      <c r="G23">
+      <c r="E23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5</v>
       </c>
@@ -9344,16 +9296,16 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24">
+        <v>61</v>
+      </c>
+      <c r="D24">
         <v>12</v>
       </c>
-      <c r="G24">
+      <c r="E24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
@@ -9361,16 +9313,16 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25">
+        <v>62</v>
+      </c>
+      <c r="D25">
         <v>15</v>
       </c>
-      <c r="G25">
+      <c r="E25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>4</v>
       </c>
@@ -9378,16 +9330,16 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26">
-        <v>11</v>
-      </c>
-      <c r="G26">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>4</v>
       </c>
@@ -9395,16 +9347,16 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27">
+        <v>61</v>
+      </c>
+      <c r="D27">
         <v>20</v>
       </c>
-      <c r="G27">
+      <c r="E27">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>4</v>
       </c>
@@ -9412,16 +9364,16 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28">
+        <v>62</v>
+      </c>
+      <c r="D28">
         <v>15</v>
       </c>
-      <c r="G28">
+      <c r="E28">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>4</v>
       </c>
@@ -9429,16 +9381,16 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29">
+        <v>60</v>
+      </c>
+      <c r="D29">
         <v>15</v>
       </c>
-      <c r="G29">
+      <c r="E29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>4</v>
       </c>
@@ -9446,16 +9398,16 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30">
+        <v>61</v>
+      </c>
+      <c r="D30">
         <v>15</v>
       </c>
-      <c r="G30">
+      <c r="E30">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>4</v>
       </c>
@@ -9463,12 +9415,12 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31">
+        <v>62</v>
+      </c>
+      <c r="D31">
         <v>8</v>
       </c>
-      <c r="G31">
+      <c r="E31">
         <v>10</v>
       </c>
     </row>
@@ -9495,7 +9447,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -9509,7 +9461,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -9523,7 +9475,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>64</v>
@@ -9537,7 +9489,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>52</v>
@@ -9551,7 +9503,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <v>64</v>
@@ -9565,7 +9517,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>56</v>
@@ -9579,7 +9531,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <v>43</v>
@@ -9593,7 +9545,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D8">
         <v>29</v>
@@ -9607,7 +9559,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D9">
         <v>32</v>
@@ -9621,7 +9573,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -9635,7 +9587,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D11">
         <v>39</v>
@@ -9649,7 +9601,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D12">
         <v>41</v>
@@ -9663,7 +9615,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>47</v>
@@ -9677,7 +9629,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <v>22</v>
@@ -9691,7 +9643,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>16</v>
@@ -9705,7 +9657,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>46</v>
@@ -9719,7 +9671,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>72</v>
@@ -9733,7 +9685,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>74</v>
@@ -9747,7 +9699,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>81</v>
@@ -9761,7 +9713,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>63</v>
@@ -9775,7 +9727,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>66</v>
@@ -9789,7 +9741,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D22">
         <v>67</v>
@@ -9803,7 +9755,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>70</v>
@@ -9817,7 +9769,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>62</v>
@@ -9831,7 +9783,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>51</v>
@@ -9845,7 +9797,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D26">
         <v>71</v>
@@ -9859,7 +9811,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>73</v>
@@ -9873,7 +9825,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D28">
         <v>83</v>
@@ -9887,7 +9839,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>64</v>
@@ -9901,7 +9853,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D30">
         <v>48</v>
@@ -9915,7 +9867,7 @@
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D31">
         <v>43</v>
@@ -9929,7 +9881,7 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D32">
         <v>39</v>
@@ -9943,7 +9895,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D33">
         <v>19</v>
@@ -9957,7 +9909,7 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>40</v>
@@ -9971,7 +9923,7 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D35">
         <v>21</v>
@@ -9985,7 +9937,7 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D36">
         <v>59</v>
@@ -9999,7 +9951,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D37">
         <v>72</v>
@@ -10013,7 +9965,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D38">
         <v>24</v>
@@ -10027,7 +9979,7 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D39">
         <v>20</v>
@@ -10041,7 +9993,7 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D40">
         <v>26</v>
@@ -10055,7 +10007,7 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D41">
         <v>15</v>
@@ -10069,7 +10021,7 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D42">
         <v>35</v>
@@ -10083,7 +10035,7 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D43">
         <v>40</v>
@@ -10097,7 +10049,7 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D44">
         <v>26</v>
@@ -10111,7 +10063,7 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D45">
         <v>26</v>
@@ -10125,7 +10077,7 @@
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D46">
         <v>35</v>
@@ -10139,7 +10091,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D47">
         <v>60</v>
@@ -10153,7 +10105,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D48">
         <v>50</v>
@@ -10167,7 +10119,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D49">
         <v>54</v>
@@ -10181,7 +10133,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D50">
         <v>63</v>
@@ -10195,7 +10147,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D51">
         <v>42</v>
@@ -10209,7 +10161,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D52">
         <v>65</v>
@@ -10223,7 +10175,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D53">
         <v>63</v>
@@ -10237,7 +10189,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D54">
         <v>47</v>
@@ -10251,7 +10203,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D55">
         <v>54</v>
@@ -10265,7 +10217,7 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D56">
         <v>67</v>
@@ -10279,7 +10231,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D57">
         <v>73</v>
@@ -10293,7 +10245,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D58">
         <v>68</v>
@@ -10307,7 +10259,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D59">
         <v>82</v>
@@ -10321,7 +10273,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D60">
         <v>81</v>
@@ -10335,7 +10287,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D61">
         <v>79</v>
@@ -10349,7 +10301,7 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>47</v>
@@ -10363,7 +10315,7 @@
         <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D63">
         <v>54</v>
@@ -10377,7 +10329,7 @@
         <v>11</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D64">
         <v>60</v>
@@ -10391,7 +10343,7 @@
         <v>11</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D65">
         <v>56</v>
@@ -10405,7 +10357,7 @@
         <v>11</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D66">
         <v>81</v>
@@ -10419,7 +10371,7 @@
         <v>11</v>
       </c>
       <c r="C67" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D67">
         <v>45</v>
@@ -10433,7 +10385,7 @@
         <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D68">
         <v>45</v>
@@ -10447,7 +10399,7 @@
         <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D69">
         <v>31</v>
@@ -10461,7 +10413,7 @@
         <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D70">
         <v>19</v>
@@ -10475,7 +10427,7 @@
         <v>11</v>
       </c>
       <c r="C71" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D71">
         <v>32</v>
@@ -10489,7 +10441,7 @@
         <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D72">
         <v>30</v>
@@ -10503,7 +10455,7 @@
         <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D73">
         <v>56</v>
@@ -10517,7 +10469,7 @@
         <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D74">
         <v>61</v>
@@ -10531,7 +10483,7 @@
         <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D75">
         <v>62</v>
@@ -10545,7 +10497,7 @@
         <v>11</v>
       </c>
       <c r="C76" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D76">
         <v>70</v>
@@ -10559,7 +10511,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D77">
         <v>74</v>
@@ -10573,7 +10525,7 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D78">
         <v>63</v>
@@ -10587,7 +10539,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D79">
         <v>61</v>
@@ -10601,7 +10553,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D80">
         <v>74</v>
@@ -10615,7 +10567,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D81">
         <v>52</v>
@@ -10629,7 +10581,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D82">
         <v>72</v>
@@ -10643,7 +10595,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D83">
         <v>62</v>
@@ -10657,7 +10609,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D84">
         <v>61</v>
@@ -10671,7 +10623,7 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D85">
         <v>52</v>
@@ -10685,7 +10637,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D86">
         <v>63</v>
@@ -10699,7 +10651,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D87">
         <v>52</v>
@@ -10713,7 +10665,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D88">
         <v>54</v>
@@ -10727,7 +10679,7 @@
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D89">
         <v>56</v>
@@ -10741,7 +10693,7 @@
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D90">
         <v>41</v>
@@ -10755,7 +10707,7 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D91">
         <v>47</v>

</xml_diff>